<commit_message>
update CiLVpUAAbP and AVMC with EU data
</commit_message>
<xml_diff>
--- a/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
+++ b/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\trans\AVMC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\trans\AVMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF646FD-413E-4B0A-A984-B8BBA1CEB9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="405" windowWidth="24435" windowHeight="16275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="405" windowWidth="24435" windowHeight="16275"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Cost Data" sheetId="16" r:id="rId2"/>
-    <sheet name="AVMC-passenger" sheetId="2" r:id="rId3"/>
-    <sheet name="AVMC-freight" sheetId="4" r:id="rId4"/>
+    <sheet name="GDP per capita adjustmentUS Dat" sheetId="17" r:id="rId3"/>
+    <sheet name="Pre GDP per capita adjustment" sheetId="18" r:id="rId4"/>
+    <sheet name="AVMC-passenger" sheetId="2" r:id="rId5"/>
+    <sheet name="AVMC-freight" sheetId="4" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Eno_TM">'[1]1997  Table 1a Modified'!#REF!</definedName>
@@ -29,7 +30,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="141">
   <si>
     <t>Sources:</t>
   </si>
@@ -443,12 +444,36 @@
   </si>
   <si>
     <t>AVMC Annual Vehicle Maintenance Cost</t>
+  </si>
+  <si>
+    <t>US Data</t>
+  </si>
+  <si>
+    <t>EU Data</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>GDP per capita</t>
+  </si>
+  <si>
+    <t>Ratio of EU:US GDP per capita</t>
+  </si>
+  <si>
+    <t>passenger</t>
+  </si>
+  <si>
+    <t>freight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="9">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -1274,7 +1299,7 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1309,149 +1334,152 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="140" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="141">
-    <cellStyle name="20% - Accent1 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Calculation 2" xfId="40" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Check Cell 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Comma 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Comma 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Comma 2 2 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Comma 2 2 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Comma 2 3" xfId="45" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Comma 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Comma 4" xfId="47" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Comma 5" xfId="48" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Comma 6" xfId="49" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Comma 7" xfId="50" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Currency 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Currency 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Currency 3 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Data" xfId="54" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Data no deci" xfId="55" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Data Superscript" xfId="56" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="57" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Good 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Heading 1 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Heading 2 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Heading 3 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Heading 4 2" xfId="63" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Hed Side" xfId="13" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Hed Side bold" xfId="64" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Hed Side Indent" xfId="65" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="66" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Hed Top" xfId="68" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="15"/>
+    <cellStyle name="20% - Accent2 2" xfId="16"/>
+    <cellStyle name="20% - Accent3 2" xfId="17"/>
+    <cellStyle name="20% - Accent4 2" xfId="18"/>
+    <cellStyle name="20% - Accent5 2" xfId="19"/>
+    <cellStyle name="20% - Accent6 2" xfId="20"/>
+    <cellStyle name="40% - Accent1 2" xfId="21"/>
+    <cellStyle name="40% - Accent2 2" xfId="22"/>
+    <cellStyle name="40% - Accent3 2" xfId="23"/>
+    <cellStyle name="40% - Accent4 2" xfId="24"/>
+    <cellStyle name="40% - Accent5 2" xfId="25"/>
+    <cellStyle name="40% - Accent6 2" xfId="26"/>
+    <cellStyle name="60% - Accent1 2" xfId="27"/>
+    <cellStyle name="60% - Accent2 2" xfId="28"/>
+    <cellStyle name="60% - Accent3 2" xfId="29"/>
+    <cellStyle name="60% - Accent4 2" xfId="30"/>
+    <cellStyle name="60% - Accent5 2" xfId="31"/>
+    <cellStyle name="60% - Accent6 2" xfId="32"/>
+    <cellStyle name="Accent1 2" xfId="33"/>
+    <cellStyle name="Accent2 2" xfId="34"/>
+    <cellStyle name="Accent3 2" xfId="35"/>
+    <cellStyle name="Accent4 2" xfId="36"/>
+    <cellStyle name="Accent5 2" xfId="37"/>
+    <cellStyle name="Accent6 2" xfId="38"/>
+    <cellStyle name="Bad 2" xfId="39"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Calculation 2" xfId="40"/>
+    <cellStyle name="Check Cell 2" xfId="41"/>
+    <cellStyle name="Comma 2" xfId="42"/>
+    <cellStyle name="Comma 2 2" xfId="11"/>
+    <cellStyle name="Comma 2 2 2" xfId="43"/>
+    <cellStyle name="Comma 2 2 3" xfId="44"/>
+    <cellStyle name="Comma 2 3" xfId="45"/>
+    <cellStyle name="Comma 3" xfId="46"/>
+    <cellStyle name="Comma 4" xfId="47"/>
+    <cellStyle name="Comma 5" xfId="48"/>
+    <cellStyle name="Comma 6" xfId="49"/>
+    <cellStyle name="Comma 7" xfId="50"/>
+    <cellStyle name="Currency 2" xfId="51"/>
+    <cellStyle name="Currency 3" xfId="52"/>
+    <cellStyle name="Currency 3 2" xfId="53"/>
+    <cellStyle name="Data" xfId="54"/>
+    <cellStyle name="Data no deci" xfId="55"/>
+    <cellStyle name="Data Superscript" xfId="56"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="57"/>
+    <cellStyle name="Explanatory Text 2" xfId="58"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Footnotes: top row" xfId="2"/>
+    <cellStyle name="Good 2" xfId="59"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
+    <cellStyle name="Heading 1 2" xfId="60"/>
+    <cellStyle name="Heading 2 2" xfId="61"/>
+    <cellStyle name="Heading 3 2" xfId="62"/>
+    <cellStyle name="Heading 4 2" xfId="63"/>
+    <cellStyle name="Hed Side" xfId="13"/>
+    <cellStyle name="Hed Side bold" xfId="64"/>
+    <cellStyle name="Hed Side Indent" xfId="65"/>
+    <cellStyle name="Hed Side Regular" xfId="66"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="67"/>
+    <cellStyle name="Hed Top" xfId="68"/>
     <cellStyle name="Hyperlink" xfId="140" builtinId="8"/>
-    <cellStyle name="Input 2" xfId="69" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Neutral 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Input 2" xfId="69"/>
+    <cellStyle name="Linked Cell 2" xfId="70"/>
+    <cellStyle name="Neutral 2" xfId="71"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="72" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Normal 11" xfId="10" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Normal 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Normal 2 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 2 3" xfId="76" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 2 4" xfId="77" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 3 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="79" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="80" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="81" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 3 3" xfId="82" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 3 4" xfId="86" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 3 5" xfId="88" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 3 6" xfId="89" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 3 7" xfId="90" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 3 8" xfId="91" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 3 9" xfId="12" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 4" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 4 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 4 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 4 2 3" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 4 3" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 4 3 3" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 4 4" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 4 4 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 4 5" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 4 6" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 4 7" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 4 8" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 5" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 5 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 5 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 6" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 7" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 8" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 9" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Note 2" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Note 2 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Output 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Percent 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Percent 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Percent 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Percent 3 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Source Hed" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Source Superscript" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Source Text" xfId="9" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="State" xfId="124" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Superscript" xfId="125" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Table Data" xfId="126" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Table Head Top" xfId="127" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Table Hed Side" xfId="128" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Title 2" xfId="129" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Title Text" xfId="130" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Title Text 1" xfId="131" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Title Text 2" xfId="132" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Title-1" xfId="14" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Title-2" xfId="133" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Title-3" xfId="134" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Total 2" xfId="135" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Warning Text 2" xfId="136" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Wrap" xfId="137" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Wrap Bold" xfId="138" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Wrap Title" xfId="139" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 10" xfId="72"/>
+    <cellStyle name="Normal 11" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="73"/>
+    <cellStyle name="Normal 2 2 2" xfId="74"/>
+    <cellStyle name="Normal 2 2 3" xfId="75"/>
+    <cellStyle name="Normal 2 3" xfId="76"/>
+    <cellStyle name="Normal 2 4" xfId="77"/>
+    <cellStyle name="Normal 3" xfId="8"/>
+    <cellStyle name="Normal 3 2" xfId="78"/>
+    <cellStyle name="Normal 3 2 2" xfId="79"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="80"/>
+    <cellStyle name="Normal 3 2 3" xfId="81"/>
+    <cellStyle name="Normal 3 3" xfId="82"/>
+    <cellStyle name="Normal 3 3 2" xfId="83"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="84"/>
+    <cellStyle name="Normal 3 3 3" xfId="85"/>
+    <cellStyle name="Normal 3 4" xfId="86"/>
+    <cellStyle name="Normal 3 4 2" xfId="87"/>
+    <cellStyle name="Normal 3 5" xfId="88"/>
+    <cellStyle name="Normal 3 6" xfId="89"/>
+    <cellStyle name="Normal 3 7" xfId="90"/>
+    <cellStyle name="Normal 3 8" xfId="91"/>
+    <cellStyle name="Normal 3 9" xfId="12"/>
+    <cellStyle name="Normal 4" xfId="92"/>
+    <cellStyle name="Normal 4 2" xfId="93"/>
+    <cellStyle name="Normal 4 2 2" xfId="94"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="95"/>
+    <cellStyle name="Normal 4 2 3" xfId="96"/>
+    <cellStyle name="Normal 4 3" xfId="97"/>
+    <cellStyle name="Normal 4 3 2" xfId="98"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="99"/>
+    <cellStyle name="Normal 4 3 3" xfId="100"/>
+    <cellStyle name="Normal 4 4" xfId="101"/>
+    <cellStyle name="Normal 4 4 2" xfId="102"/>
+    <cellStyle name="Normal 4 5" xfId="103"/>
+    <cellStyle name="Normal 4 6" xfId="104"/>
+    <cellStyle name="Normal 4 7" xfId="105"/>
+    <cellStyle name="Normal 4 8" xfId="106"/>
+    <cellStyle name="Normal 5" xfId="107"/>
+    <cellStyle name="Normal 5 2" xfId="108"/>
+    <cellStyle name="Normal 5 3" xfId="109"/>
+    <cellStyle name="Normal 6" xfId="110"/>
+    <cellStyle name="Normal 6 2" xfId="111"/>
+    <cellStyle name="Normal 7" xfId="112"/>
+    <cellStyle name="Normal 8" xfId="113"/>
+    <cellStyle name="Normal 9" xfId="114"/>
+    <cellStyle name="Note 2" xfId="115"/>
+    <cellStyle name="Note 2 2" xfId="116"/>
+    <cellStyle name="Output 2" xfId="117"/>
+    <cellStyle name="Parent row" xfId="3"/>
+    <cellStyle name="Percent 2" xfId="118"/>
+    <cellStyle name="Percent 2 2" xfId="119"/>
+    <cellStyle name="Percent 3" xfId="120"/>
+    <cellStyle name="Percent 3 2" xfId="121"/>
+    <cellStyle name="Source Hed" xfId="122"/>
+    <cellStyle name="Source Superscript" xfId="123"/>
+    <cellStyle name="Source Text" xfId="9"/>
+    <cellStyle name="State" xfId="124"/>
+    <cellStyle name="Superscript" xfId="125"/>
+    <cellStyle name="Table Data" xfId="126"/>
+    <cellStyle name="Table Head Top" xfId="127"/>
+    <cellStyle name="Table Hed Side" xfId="128"/>
+    <cellStyle name="Table title" xfId="7"/>
+    <cellStyle name="Title 2" xfId="129"/>
+    <cellStyle name="Title Text" xfId="130"/>
+    <cellStyle name="Title Text 1" xfId="131"/>
+    <cellStyle name="Title Text 2" xfId="132"/>
+    <cellStyle name="Title-1" xfId="14"/>
+    <cellStyle name="Title-2" xfId="133"/>
+    <cellStyle name="Title-3" xfId="134"/>
+    <cellStyle name="Total 2" xfId="135"/>
+    <cellStyle name="Warning Text 2" xfId="136"/>
+    <cellStyle name="Wrap" xfId="137"/>
+    <cellStyle name="Wrap Bold" xfId="138"/>
+    <cellStyle name="Wrap Title" xfId="139"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1623,23 +1651,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1675,23 +1686,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1867,14 +1861,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="2" max="2" width="73.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2202,15 +2198,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{F7E7A3DE-93B2-4E97-8034-BE9FA2CBB032}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{0A5F8456-85E2-4B46-98CB-42301965587F}"/>
-    <hyperlink ref="B28" r:id="rId3" display="https://www.icao.int/MID/Documents/2017/Aviation Data and Analysis Seminar/PPT3 - Airlines Operating costs and productivity.pdf" xr:uid="{32C07062-31D6-4D64-9941-54355C398A54}"/>
-    <hyperlink ref="B21" r:id="rId4" xr:uid="{A1682FDD-C2BD-495E-8A6B-5F03193720A5}"/>
-    <hyperlink ref="B35" r:id="rId5" xr:uid="{86CB5594-D53D-4996-A0D1-BB39C7D7D625}"/>
-    <hyperlink ref="B41" r:id="rId6" xr:uid="{B0ED8C7C-30CE-4966-BD3F-14CBF2AB2A2B}"/>
-    <hyperlink ref="B48" r:id="rId7" xr:uid="{B27ABC8E-899E-48AC-8608-F37B2EDFED93}"/>
-    <hyperlink ref="B55" r:id="rId8" display="http://www.sparusa.com/Presentations/Presentation-Commercial Ship Life Cycle &amp; Required Freight Rate (RFR) Cost Model.pdf" xr:uid="{4BC70352-C238-4681-9474-B434C82A9EE6}"/>
-    <hyperlink ref="B62" r:id="rId9" xr:uid="{5439DEF3-45BA-42A3-B033-B27D7C2B3817}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B28" r:id="rId3" display="https://www.icao.int/MID/Documents/2017/Aviation Data and Analysis Seminar/PPT3 - Airlines Operating costs and productivity.pdf"/>
+    <hyperlink ref="B21" r:id="rId4"/>
+    <hyperlink ref="B35" r:id="rId5"/>
+    <hyperlink ref="B41" r:id="rId6"/>
+    <hyperlink ref="B48" r:id="rId7"/>
+    <hyperlink ref="B55" r:id="rId8" display="http://www.sparusa.com/Presentations/Presentation-Commercial Ship Life Cycle &amp; Required Freight Rate (RFR) Cost Model.pdf"/>
+    <hyperlink ref="B62" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -2218,16 +2214,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA56E7A-E0B4-48E9-AA66-C39B91D43ABA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.59765625" customWidth="1"/>
+    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3021,9 +3017,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{DEA7D659-12AB-4A56-889B-D770D6477AD9}"/>
-    <hyperlink ref="B13" r:id="rId2" xr:uid="{83856772-5164-484D-9C39-5E905DAB68CE}"/>
-    <hyperlink ref="A65" r:id="rId3" xr:uid="{CF3217FC-13DF-41C0-A64F-4474765B54A2}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId2"/>
+    <hyperlink ref="A65" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -3031,22 +3027,1521 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:AG15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.9296875" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33">
+      <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="B2">
+        <v>2019</v>
+      </c>
+      <c r="C2">
+        <v>2020</v>
+      </c>
+      <c r="D2">
+        <v>2021</v>
+      </c>
+      <c r="E2">
+        <v>2022</v>
+      </c>
+      <c r="F2">
+        <v>2023</v>
+      </c>
+      <c r="G2">
+        <v>2024</v>
+      </c>
+      <c r="H2">
+        <v>2025</v>
+      </c>
+      <c r="I2">
+        <v>2026</v>
+      </c>
+      <c r="J2">
+        <v>2027</v>
+      </c>
+      <c r="K2">
+        <v>2028</v>
+      </c>
+      <c r="L2">
+        <v>2029</v>
+      </c>
+      <c r="M2">
+        <v>2030</v>
+      </c>
+      <c r="N2">
+        <v>2031</v>
+      </c>
+      <c r="O2">
+        <v>2032</v>
+      </c>
+      <c r="P2">
+        <v>2033</v>
+      </c>
+      <c r="Q2">
+        <v>2034</v>
+      </c>
+      <c r="R2">
+        <v>2035</v>
+      </c>
+      <c r="S2">
+        <v>2036</v>
+      </c>
+      <c r="T2">
+        <v>2037</v>
+      </c>
+      <c r="U2">
+        <v>2038</v>
+      </c>
+      <c r="V2">
+        <v>2039</v>
+      </c>
+      <c r="W2">
+        <v>2040</v>
+      </c>
+      <c r="X2">
+        <v>2041</v>
+      </c>
+      <c r="Y2">
+        <v>2042</v>
+      </c>
+      <c r="Z2">
+        <v>2043</v>
+      </c>
+      <c r="AA2">
+        <v>2044</v>
+      </c>
+      <c r="AB2">
+        <v>2045</v>
+      </c>
+      <c r="AC2">
+        <v>2046</v>
+      </c>
+      <c r="AD2">
+        <v>2047</v>
+      </c>
+      <c r="AE2">
+        <v>2048</v>
+      </c>
+      <c r="AF2">
+        <v>2049</v>
+      </c>
+      <c r="AG2">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3">
+        <v>514346446</v>
+      </c>
+      <c r="C3">
+        <v>514610000</v>
+      </c>
+      <c r="D3">
+        <v>514723000</v>
+      </c>
+      <c r="E3">
+        <v>514707000</v>
+      </c>
+      <c r="F3">
+        <v>514601000</v>
+      </c>
+      <c r="G3">
+        <v>514433000</v>
+      </c>
+      <c r="H3">
+        <v>514244000</v>
+      </c>
+      <c r="I3">
+        <v>514023000</v>
+      </c>
+      <c r="J3">
+        <v>513759000</v>
+      </c>
+      <c r="K3">
+        <v>513445000</v>
+      </c>
+      <c r="L3">
+        <v>513064000</v>
+      </c>
+      <c r="M3">
+        <v>512622000</v>
+      </c>
+      <c r="N3">
+        <v>512121000</v>
+      </c>
+      <c r="O3">
+        <v>511577000</v>
+      </c>
+      <c r="P3">
+        <v>510981000</v>
+      </c>
+      <c r="Q3">
+        <v>510344000</v>
+      </c>
+      <c r="R3">
+        <v>509670000</v>
+      </c>
+      <c r="S3">
+        <v>508960000</v>
+      </c>
+      <c r="T3">
+        <v>508219000</v>
+      </c>
+      <c r="U3">
+        <v>507438000</v>
+      </c>
+      <c r="V3">
+        <v>506618000</v>
+      </c>
+      <c r="W3">
+        <v>505751000</v>
+      </c>
+      <c r="X3">
+        <v>504841000</v>
+      </c>
+      <c r="Y3">
+        <v>503886000</v>
+      </c>
+      <c r="Z3">
+        <v>502879000</v>
+      </c>
+      <c r="AA3">
+        <v>501821000</v>
+      </c>
+      <c r="AB3">
+        <v>500708000</v>
+      </c>
+      <c r="AC3">
+        <v>499546000</v>
+      </c>
+      <c r="AD3">
+        <v>498338000</v>
+      </c>
+      <c r="AE3">
+        <v>497082000</v>
+      </c>
+      <c r="AF3">
+        <v>495789000</v>
+      </c>
+      <c r="AG3">
+        <v>494402000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4">
+        <v>20559765530949.57</v>
+      </c>
+      <c r="C4">
+        <v>20856287742024.746</v>
+      </c>
+      <c r="D4">
+        <v>21135822055400.117</v>
+      </c>
+      <c r="E4">
+        <v>21422361892194.555</v>
+      </c>
+      <c r="F4">
+        <v>21722424737854.797</v>
+      </c>
+      <c r="G4">
+        <v>22038622615670.715</v>
+      </c>
+      <c r="H4">
+        <v>22370875805160.238</v>
+      </c>
+      <c r="I4">
+        <v>22716255772502.805</v>
+      </c>
+      <c r="J4">
+        <v>23072297969104.27</v>
+      </c>
+      <c r="K4">
+        <v>23437805243577.699</v>
+      </c>
+      <c r="L4">
+        <v>23811879426396.098</v>
+      </c>
+      <c r="M4">
+        <v>24193806847127.551</v>
+      </c>
+      <c r="N4">
+        <v>24583211863297.754</v>
+      </c>
+      <c r="O4">
+        <v>24980005356259.531</v>
+      </c>
+      <c r="P4">
+        <v>25384387288368.004</v>
+      </c>
+      <c r="Q4">
+        <v>25796741552812.211</v>
+      </c>
+      <c r="R4">
+        <v>26217530834374.805</v>
+      </c>
+      <c r="S4">
+        <v>26647364440142.484</v>
+      </c>
+      <c r="T4">
+        <v>27085768156188.129</v>
+      </c>
+      <c r="U4">
+        <v>27533234337083.137</v>
+      </c>
+      <c r="V4">
+        <v>27990230290196.063</v>
+      </c>
+      <c r="W4">
+        <v>28457321227734.191</v>
+      </c>
+      <c r="X4">
+        <v>28935201717812.43</v>
+      </c>
+      <c r="Y4">
+        <v>29425750103939.48</v>
+      </c>
+      <c r="Z4">
+        <v>29929672100891.195</v>
+      </c>
+      <c r="AA4">
+        <v>30447563585120.621</v>
+      </c>
+      <c r="AB4">
+        <v>30979778539609.855</v>
+      </c>
+      <c r="AC4">
+        <v>31526785965582.813</v>
+      </c>
+      <c r="AD4">
+        <v>32088090645306.137</v>
+      </c>
+      <c r="AE4">
+        <v>32664160345128.531</v>
+      </c>
+      <c r="AF4">
+        <v>33255473464439.008</v>
+      </c>
+      <c r="AG4">
+        <v>33862541066714.402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6">
+        <f>B4/B3</f>
+        <v>39972.601523428377</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:AG6" si="0">C4/C3</f>
+        <v>40528.337463369826</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>41062.517228490113</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>41620.498443181372</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>42212.169696239995</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>42840.608234057137</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>43502.453709056863</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>44193.072630023955</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>44908.795698185859</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>45648.132211975382</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>46411.128877481366</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>47196.192998208331</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>48002.741272663596</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>48829.414450335986</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>49677.751791882678</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>50547.751228215107</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>51440.208045156287</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>52356.500393238144</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>53295.465451287986</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>54259.307219962117</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="0"/>
+        <v>55249.182402117694</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="0"/>
+        <v>56267.454197291139</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="0"/>
+        <v>57315.475006610854</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>58397.633798000898</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>59516.647346362035</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="0"/>
+        <v>60674.151908988708</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="0"/>
+        <v>61871.946403112903</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="0"/>
+        <v>63110.876607124897</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="0"/>
+        <v>64390.214363155399</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="0"/>
+        <v>65711.814841673069</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="0"/>
+        <v>67075.859820284444</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="0"/>
+        <v>68491.917643363908</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" s="14"/>
+      <c r="B9">
+        <v>2019</v>
+      </c>
+      <c r="C9">
+        <v>2020</v>
+      </c>
+      <c r="D9">
+        <v>2021</v>
+      </c>
+      <c r="E9">
+        <v>2022</v>
+      </c>
+      <c r="F9">
+        <v>2023</v>
+      </c>
+      <c r="G9">
+        <v>2024</v>
+      </c>
+      <c r="H9">
+        <v>2025</v>
+      </c>
+      <c r="I9">
+        <v>2026</v>
+      </c>
+      <c r="J9">
+        <v>2027</v>
+      </c>
+      <c r="K9">
+        <v>2028</v>
+      </c>
+      <c r="L9">
+        <v>2029</v>
+      </c>
+      <c r="M9">
+        <v>2030</v>
+      </c>
+      <c r="N9">
+        <v>2031</v>
+      </c>
+      <c r="O9">
+        <v>2032</v>
+      </c>
+      <c r="P9">
+        <v>2033</v>
+      </c>
+      <c r="Q9">
+        <v>2034</v>
+      </c>
+      <c r="R9">
+        <v>2035</v>
+      </c>
+      <c r="S9">
+        <v>2036</v>
+      </c>
+      <c r="T9">
+        <v>2037</v>
+      </c>
+      <c r="U9">
+        <v>2038</v>
+      </c>
+      <c r="V9">
+        <v>2039</v>
+      </c>
+      <c r="W9">
+        <v>2040</v>
+      </c>
+      <c r="X9">
+        <v>2041</v>
+      </c>
+      <c r="Y9">
+        <v>2042</v>
+      </c>
+      <c r="Z9">
+        <v>2043</v>
+      </c>
+      <c r="AA9">
+        <v>2044</v>
+      </c>
+      <c r="AB9">
+        <v>2045</v>
+      </c>
+      <c r="AC9">
+        <v>2046</v>
+      </c>
+      <c r="AD9">
+        <v>2047</v>
+      </c>
+      <c r="AE9">
+        <v>2048</v>
+      </c>
+      <c r="AF9">
+        <v>2049</v>
+      </c>
+      <c r="AG9">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10">
+        <v>330268840</v>
+      </c>
+      <c r="C10">
+        <v>332639102</v>
+      </c>
+      <c r="D10">
+        <v>334998398</v>
+      </c>
+      <c r="E10">
+        <v>337341954</v>
+      </c>
+      <c r="F10">
+        <v>339665118</v>
+      </c>
+      <c r="G10">
+        <v>341963408</v>
+      </c>
+      <c r="H10">
+        <v>344234377</v>
+      </c>
+      <c r="I10">
+        <v>346481182</v>
+      </c>
+      <c r="J10">
+        <v>348695115</v>
+      </c>
+      <c r="K10">
+        <v>350872007</v>
+      </c>
+      <c r="L10">
+        <v>353008224</v>
+      </c>
+      <c r="M10">
+        <v>355100730</v>
+      </c>
+      <c r="N10">
+        <v>357147329</v>
+      </c>
+      <c r="O10">
+        <v>359146709</v>
+      </c>
+      <c r="P10">
+        <v>361098559</v>
+      </c>
+      <c r="Q10">
+        <v>363003410</v>
+      </c>
+      <c r="R10">
+        <v>364862145</v>
+      </c>
+      <c r="S10">
+        <v>366676312</v>
+      </c>
+      <c r="T10">
+        <v>368447857</v>
+      </c>
+      <c r="U10">
+        <v>370178704</v>
+      </c>
+      <c r="V10">
+        <v>371871238</v>
+      </c>
+      <c r="W10">
+        <v>373527973</v>
+      </c>
+      <c r="X10">
+        <v>375151805</v>
+      </c>
+      <c r="Y10">
+        <v>376746115</v>
+      </c>
+      <c r="Z10">
+        <v>378314343</v>
+      </c>
+      <c r="AA10">
+        <v>379860859</v>
+      </c>
+      <c r="AB10">
+        <v>381390297</v>
+      </c>
+      <c r="AC10">
+        <v>382907447</v>
+      </c>
+      <c r="AD10">
+        <v>384415207</v>
+      </c>
+      <c r="AE10">
+        <v>385917628</v>
+      </c>
+      <c r="AF10">
+        <v>387418788</v>
+      </c>
+      <c r="AG10">
+        <v>388922201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11">
+        <v>19260564565319.313</v>
+      </c>
+      <c r="C11">
+        <v>19570694229280.551</v>
+      </c>
+      <c r="D11">
+        <v>19846925958285.945</v>
+      </c>
+      <c r="E11">
+        <v>20136856085592.691</v>
+      </c>
+      <c r="F11">
+        <v>20449876595278.277</v>
+      </c>
+      <c r="G11">
+        <v>20785071453021.242</v>
+      </c>
+      <c r="H11">
+        <v>21137860487214.293</v>
+      </c>
+      <c r="I11">
+        <v>21504884905345.414</v>
+      </c>
+      <c r="J11">
+        <v>21883765124004.84</v>
+      </c>
+      <c r="K11">
+        <v>22272742778460.578</v>
+      </c>
+      <c r="L11">
+        <v>22670459610925.633</v>
+      </c>
+      <c r="M11">
+        <v>23076094349249.734</v>
+      </c>
+      <c r="N11">
+        <v>23489489056480.902</v>
+      </c>
+      <c r="O11">
+        <v>23911159659995.598</v>
+      </c>
+      <c r="P11">
+        <v>24342022194115.273</v>
+      </c>
+      <c r="Q11">
+        <v>24783055867942.18</v>
+      </c>
+      <c r="R11">
+        <v>25235197774058.039</v>
+      </c>
+      <c r="S11">
+        <v>25699353417654.18</v>
+      </c>
+      <c r="T11">
+        <v>26176480949572.586</v>
+      </c>
+      <c r="U11">
+        <v>26667317408922.48</v>
+      </c>
+      <c r="V11">
+        <v>27172315548299.516</v>
+      </c>
+      <c r="W11">
+        <v>27691759654217.266</v>
+      </c>
+      <c r="X11">
+        <v>28225881367538.613</v>
+      </c>
+      <c r="Y11">
+        <v>28774996562167.52</v>
+      </c>
+      <c r="Z11">
+        <v>29339157883754.633</v>
+      </c>
+      <c r="AA11">
+        <v>29918091574916.535</v>
+      </c>
+      <c r="AB11">
+        <v>30511365941317.828</v>
+      </c>
+      <c r="AC11">
+        <v>31118686167314.816</v>
+      </c>
+      <c r="AD11">
+        <v>31739925903345.926</v>
+      </c>
+      <c r="AE11">
+        <v>32374800862897.605</v>
+      </c>
+      <c r="AF11">
+        <v>33022858293374.176</v>
+      </c>
+      <c r="AG11">
+        <v>33683645442179.992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13">
+        <f>B11/B10</f>
+        <v>58317.837569294497</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:AG13" si="1">C11/C10</f>
+        <v>58834.61719205985</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>59244.838413483834</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>59692.711940574969</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>60205.995586742225</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>60781.566000246559</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>61405.431588299194</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>62066.530658930315</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>62759.024094744891</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>63478.255130397389</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>64220.769006575982</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>64984.643510166068</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>65769.745842004893</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>66577.693908356538</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>67411.020031556734</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>68272.239833620784</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>69163.650216599039</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="1"/>
+        <v>70087.302006174257</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>71045.279412692005</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="1"/>
+        <v>72039.037148183648</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="1"/>
+        <v>73069.150748086395</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="1"/>
+        <v>74135.705103449553</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="1"/>
+        <v>75238.559408073794</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="1"/>
+        <v>76377.686236173977</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="1"/>
+        <v>77552.327651914151</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="1"/>
+        <v>78760.65897833537</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="1"/>
+        <v>80000.372797417629</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="1"/>
+        <v>81269.472325814582</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="1"/>
+        <v>82566.780203744449</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="1"/>
+        <v>83890.443229241675</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="1"/>
+        <v>85238.143621919997</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="1"/>
+        <v>86607.669491667795</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="28.5">
+      <c r="A15" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15">
+        <f>B6/B13</f>
+        <v>0.68542667543068758</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:AG15" si="2">C6/C13</f>
+        <v>0.68885189362359633</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.69309864501452478</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0.69724589636026646</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0.70112900359603725</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0.70482896465489808</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>0.70844634723398403</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0.71202743509017652</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>0.71557511204107915</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0.71911447657476935</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>0.72268098927200686</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>0.72626686012096153</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>0.72986052565837778</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>0.73342003280481805</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="2"/>
+        <v>0.7369381411025574</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="2"/>
+        <v>0.74038513093169056</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="2"/>
+        <v>0.74374628701726353</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>0.74701834561452884</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>0.75016195153096865</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="2"/>
+        <v>0.75319312095123114</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="2"/>
+        <v>0.75612186314570806</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="2"/>
+        <v>0.75897914667129807</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="2"/>
+        <v>0.76178325924273838</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="2"/>
+        <v>0.76459024455682745</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="2"/>
+        <v>0.76743856887824879</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="2"/>
+        <v>0.77036115106246505</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="2"/>
+        <v>0.7733957260397929</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="2"/>
+        <v>0.77656313989722126</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="2"/>
+        <v>0.77985618676499224</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="2"/>
+        <v>0.78330513360272624</v>
+      </c>
+      <c r="AF15">
+        <f t="shared" si="2"/>
+        <v>0.78692304841602734</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="2"/>
+        <v>0.79082970417479326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <f>'Cost Data'!$C85</f>
+        <v>344.72326776048766</v>
+      </c>
+      <c r="C3" s="5">
+        <f>'Cost Data'!$B85</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="D3" s="5">
+        <f>'Cost Data'!$B85</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="E3" s="5">
+        <f>'Cost Data'!$B85</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="F3" s="5">
+        <f>'Cost Data'!$B85</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="G3" s="5">
+        <f>'Cost Data'!$B85</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="H3" s="5">
+        <f>'Cost Data'!$C85</f>
+        <v>344.72326776048766</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <f>'Cost Data'!$C86</f>
+        <v>1950.9181132216977</v>
+      </c>
+      <c r="C4" s="5">
+        <f>'Cost Data'!$B86</f>
+        <v>2482.986689554888</v>
+      </c>
+      <c r="D4" s="5">
+        <f>'Cost Data'!$B86</f>
+        <v>2482.986689554888</v>
+      </c>
+      <c r="E4" s="5">
+        <f>'Cost Data'!$B86</f>
+        <v>2482.986689554888</v>
+      </c>
+      <c r="F4" s="5">
+        <f>'Cost Data'!$B86</f>
+        <v>2482.986689554888</v>
+      </c>
+      <c r="G4" s="5">
+        <f>'Cost Data'!$B86</f>
+        <v>2482.986689554888</v>
+      </c>
+      <c r="H4" s="5">
+        <f>'Cost Data'!$C86</f>
+        <v>1950.9181132216977</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="26">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <f>'Cost Data'!$B87</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="D5" s="5">
+        <f>'Cost Data'!$B87</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="E5" s="5">
+        <f>'Cost Data'!$B87</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="F5" s="5">
+        <f>'Cost Data'!$B87</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="G5" s="5">
+        <f>'Cost Data'!$B87</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="H5" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <f>'Cost Data'!$C88</f>
+        <v>2434118.0622207024</v>
+      </c>
+      <c r="C6" s="5">
+        <f>'Cost Data'!$B88</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="D6" s="5">
+        <f>'Cost Data'!$B88</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="E6" s="5">
+        <f>'Cost Data'!$B88</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="F6" s="5">
+        <f>'Cost Data'!$B88</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="G6" s="5">
+        <f>'Cost Data'!$B88</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="H6" s="5">
+        <f>'Cost Data'!$C88</f>
+        <v>2434118.0622207024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="26">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <f>'Cost Data'!$B89</f>
+        <v>3000</v>
+      </c>
+      <c r="D7" s="5">
+        <f>'Cost Data'!$B89</f>
+        <v>3000</v>
+      </c>
+      <c r="E7" s="5">
+        <f>'Cost Data'!$B89</f>
+        <v>3000</v>
+      </c>
+      <c r="F7" s="5">
+        <f>'Cost Data'!$B89</f>
+        <v>3000</v>
+      </c>
+      <c r="G7" s="5">
+        <f>'Cost Data'!$B89</f>
+        <v>3000</v>
+      </c>
+      <c r="H7" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <f>'Cost Data'!$C90</f>
+        <v>480.24283381885334</v>
+      </c>
+      <c r="C8" s="5">
+        <f>'Cost Data'!$B90</f>
+        <v>914.32735845675347</v>
+      </c>
+      <c r="D8" s="5">
+        <f>'Cost Data'!$B90</f>
+        <v>914.32735845675347</v>
+      </c>
+      <c r="E8" s="5">
+        <f>'Cost Data'!$B90</f>
+        <v>914.32735845675347</v>
+      </c>
+      <c r="F8" s="5">
+        <f>'Cost Data'!$B90</f>
+        <v>914.32735845675347</v>
+      </c>
+      <c r="G8" s="5">
+        <f>'Cost Data'!$B90</f>
+        <v>914.32735845675347</v>
+      </c>
+      <c r="H8" s="5">
+        <f>'Cost Data'!$C90</f>
+        <v>480.24283381885334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6">
+        <f>'Cost Data'!$C94</f>
+        <v>344.72326776048766</v>
+      </c>
+      <c r="C12" s="6">
+        <f>'Cost Data'!$B94</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="D12" s="6">
+        <f>'Cost Data'!$B94</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="E12" s="6">
+        <f>'Cost Data'!$B94</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="F12" s="6">
+        <f>'Cost Data'!$B94</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="G12" s="6">
+        <f>'Cost Data'!$B94</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="H12" s="6">
+        <f>'Cost Data'!$C94</f>
+        <v>344.72326776048766</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6">
+        <f>'Cost Data'!$C95</f>
+        <v>11785.714285714286</v>
+      </c>
+      <c r="C13" s="6">
+        <f>'Cost Data'!$B95</f>
+        <v>15000</v>
+      </c>
+      <c r="D13" s="6">
+        <f>'Cost Data'!$B95</f>
+        <v>15000</v>
+      </c>
+      <c r="E13" s="6">
+        <f>'Cost Data'!$B95</f>
+        <v>15000</v>
+      </c>
+      <c r="F13" s="6">
+        <f>'Cost Data'!$B95</f>
+        <v>15000</v>
+      </c>
+      <c r="G13" s="6">
+        <f>'Cost Data'!$B95</f>
+        <v>15000</v>
+      </c>
+      <c r="H13" s="6">
+        <f>'Cost Data'!$C95</f>
+        <v>11785.714285714286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="26">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6">
+        <f>'Cost Data'!$B96</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="D14" s="6">
+        <f>'Cost Data'!$B96</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="E14" s="6">
+        <f>'Cost Data'!$B96</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="F14" s="6">
+        <f>'Cost Data'!$B96</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="G14" s="6">
+        <f>'Cost Data'!$B96</f>
+        <v>2279318.9754813975</v>
+      </c>
+      <c r="H14" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="6">
+        <f>'Cost Data'!$C97</f>
+        <v>2434118.0622207024</v>
+      </c>
+      <c r="C15" s="6">
+        <f>'Cost Data'!$B97</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="D15" s="6">
+        <f>'Cost Data'!$B97</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="E15" s="6">
+        <f>'Cost Data'!$B97</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="F15" s="6">
+        <f>'Cost Data'!$B97</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="G15" s="6">
+        <f>'Cost Data'!$B97</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="H15" s="6">
+        <f>'Cost Data'!$C97</f>
+        <v>2434118.0622207024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="26">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <f>'Cost Data'!$B98</f>
+        <v>1695890</v>
+      </c>
+      <c r="D16" s="6">
+        <f>'Cost Data'!$B98</f>
+        <v>1695890</v>
+      </c>
+      <c r="E16" s="6">
+        <f>'Cost Data'!$B98</f>
+        <v>1695890</v>
+      </c>
+      <c r="F16" s="6">
+        <f>'Cost Data'!$B98</f>
+        <v>1695890</v>
+      </c>
+      <c r="G16" s="6">
+        <f>'Cost Data'!$B98</f>
+        <v>1695890</v>
+      </c>
+      <c r="H16" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="26">
+        <v>0</v>
+      </c>
+      <c r="C17" s="26">
+        <v>0</v>
+      </c>
+      <c r="D17" s="26">
+        <v>0</v>
+      </c>
+      <c r="E17" s="26">
+        <v>0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>0</v>
+      </c>
+      <c r="G17" s="26">
+        <v>0</v>
+      </c>
+      <c r="H17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="8" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="8" width="23.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3080,32 +4575,32 @@
         <v>2</v>
       </c>
       <c r="B2" s="5">
-        <f>'Cost Data'!$C85</f>
-        <v>344.72326776048766</v>
+        <f>'Pre GDP per capita adjustment'!B3*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>236.28252336467378</v>
       </c>
       <c r="C2" s="5">
-        <f>'Cost Data'!$B85</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!C3*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="D2" s="5">
-        <f>'Cost Data'!$B85</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!D3*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="E2" s="5">
-        <f>'Cost Data'!$B85</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!E3*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="F2" s="5">
-        <f>'Cost Data'!$B85</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!F3*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="G2" s="5">
-        <f>'Cost Data'!$B85</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!G3*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="H2" s="5">
-        <f>'Cost Data'!$C85</f>
-        <v>344.72326776048766</v>
+        <f>'Pre GDP per capita adjustment'!H3*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>236.28252336467378</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3113,62 +4608,64 @@
         <v>3</v>
       </c>
       <c r="B3" s="5">
-        <f>'Cost Data'!$C86</f>
-        <v>1950.9181132216977</v>
+        <f>'Pre GDP per capita adjustment'!B4*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1337.2113163830579</v>
       </c>
       <c r="C3" s="5">
-        <f>'Cost Data'!$B86</f>
-        <v>2482.986689554888</v>
+        <f>'Pre GDP per capita adjustment'!C4*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1701.9053117602557</v>
       </c>
       <c r="D3" s="5">
-        <f>'Cost Data'!$B86</f>
-        <v>2482.986689554888</v>
+        <f>'Pre GDP per capita adjustment'!D4*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1701.9053117602557</v>
       </c>
       <c r="E3" s="5">
-        <f>'Cost Data'!$B86</f>
-        <v>2482.986689554888</v>
+        <f>'Pre GDP per capita adjustment'!E4*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1701.9053117602557</v>
       </c>
       <c r="F3" s="5">
-        <f>'Cost Data'!$B86</f>
-        <v>2482.986689554888</v>
+        <f>'Pre GDP per capita adjustment'!F4*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1701.9053117602557</v>
       </c>
       <c r="G3" s="5">
-        <f>'Cost Data'!$B86</f>
-        <v>2482.986689554888</v>
+        <f>'Pre GDP per capita adjustment'!G4*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1701.9053117602557</v>
       </c>
       <c r="H3" s="5">
-        <f>'Cost Data'!$C86</f>
-        <v>1950.9181132216977</v>
+        <f>'Pre GDP per capita adjustment'!H4*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1337.2113163830579</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="5">
+        <f>'Pre GDP per capita adjustment'!B5*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <f>'Cost Data'!$B87</f>
-        <v>2279318.9754813975</v>
+        <f>'Pre GDP per capita adjustment'!C5*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
       </c>
       <c r="D4" s="5">
-        <f>'Cost Data'!$B87</f>
-        <v>2279318.9754813975</v>
+        <f>'Pre GDP per capita adjustment'!D5*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
       </c>
       <c r="E4" s="5">
-        <f>'Cost Data'!$B87</f>
-        <v>2279318.9754813975</v>
+        <f>'Pre GDP per capita adjustment'!E5*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
       </c>
       <c r="F4" s="5">
-        <f>'Cost Data'!$B87</f>
-        <v>2279318.9754813975</v>
+        <f>'Pre GDP per capita adjustment'!F5*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
       </c>
       <c r="G4" s="5">
-        <f>'Cost Data'!$B87</f>
-        <v>2279318.9754813975</v>
-      </c>
-      <c r="H4" s="26">
+        <f>'Pre GDP per capita adjustment'!G5*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
+      </c>
+      <c r="H4" s="5">
+        <f>'Pre GDP per capita adjustment'!H5*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
     </row>
@@ -3177,62 +4674,64 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <f>'Cost Data'!$C88</f>
-        <v>2434118.0622207024</v>
+        <f>'Pre GDP per capita adjustment'!B6*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1668409.4509937237</v>
       </c>
       <c r="C5" s="5">
-        <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!C6*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="D5" s="5">
-        <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!D6*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="E5" s="5">
-        <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!E6*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="F5" s="5">
-        <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!F6*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="G5" s="5">
-        <f>'Cost Data'!$B88</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!G6*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="H5" s="5">
-        <f>'Cost Data'!$C88</f>
-        <v>2434118.0622207024</v>
+        <f>'Pre GDP per capita adjustment'!H6*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1668409.4509937237</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="5">
+        <f>'Pre GDP per capita adjustment'!B7*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
       <c r="C6" s="5">
-        <f>'Cost Data'!$B89</f>
-        <v>3000</v>
+        <f>'Pre GDP per capita adjustment'!C7*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2056.2800262920628</v>
       </c>
       <c r="D6" s="5">
-        <f>'Cost Data'!$B89</f>
-        <v>3000</v>
+        <f>'Pre GDP per capita adjustment'!D7*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2056.2800262920628</v>
       </c>
       <c r="E6" s="5">
-        <f>'Cost Data'!$B89</f>
-        <v>3000</v>
+        <f>'Pre GDP per capita adjustment'!E7*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2056.2800262920628</v>
       </c>
       <c r="F6" s="5">
-        <f>'Cost Data'!$B89</f>
-        <v>3000</v>
+        <f>'Pre GDP per capita adjustment'!F7*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2056.2800262920628</v>
       </c>
       <c r="G6" s="5">
-        <f>'Cost Data'!$B89</f>
-        <v>3000</v>
-      </c>
-      <c r="H6" s="26">
+        <f>'Pre GDP per capita adjustment'!G7*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2056.2800262920628</v>
+      </c>
+      <c r="H6" s="5">
+        <f>'Pre GDP per capita adjustment'!H7*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
     </row>
@@ -3241,32 +4740,32 @@
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <f>'Cost Data'!$C90</f>
-        <v>480.24283381885334</v>
+        <f>'Pre GDP per capita adjustment'!B8*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>329.17124898386885</v>
       </c>
       <c r="C7" s="5">
-        <f>'Cost Data'!$B90</f>
-        <v>914.32735845675347</v>
+        <f>'Pre GDP per capita adjustment'!C8*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>626.70436156233507</v>
       </c>
       <c r="D7" s="5">
-        <f>'Cost Data'!$B90</f>
-        <v>914.32735845675347</v>
+        <f>'Pre GDP per capita adjustment'!D8*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>626.70436156233507</v>
       </c>
       <c r="E7" s="5">
-        <f>'Cost Data'!$B90</f>
-        <v>914.32735845675347</v>
+        <f>'Pre GDP per capita adjustment'!E8*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>626.70436156233507</v>
       </c>
       <c r="F7" s="5">
-        <f>'Cost Data'!$B90</f>
-        <v>914.32735845675347</v>
+        <f>'Pre GDP per capita adjustment'!F8*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>626.70436156233507</v>
       </c>
       <c r="G7" s="5">
-        <f>'Cost Data'!$B90</f>
-        <v>914.32735845675347</v>
+        <f>'Pre GDP per capita adjustment'!G8*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>626.70436156233507</v>
       </c>
       <c r="H7" s="5">
-        <f>'Cost Data'!$C90</f>
-        <v>480.24283381885334</v>
+        <f>'Pre GDP per capita adjustment'!H8*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>329.17124898386885</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3287,23 +4786,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="8" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="8" width="23.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3337,32 +4838,32 @@
         <v>2</v>
       </c>
       <c r="B2" s="6">
-        <f>'Cost Data'!$C94</f>
-        <v>344.72326776048766</v>
+        <f>'Pre GDP per capita adjustment'!B12*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>236.28252336467378</v>
       </c>
       <c r="C2" s="6">
-        <f>'Cost Data'!$B94</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!C12*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="D2" s="6">
-        <f>'Cost Data'!$B94</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!D12*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="E2" s="6">
-        <f>'Cost Data'!$B94</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!E12*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="F2" s="6">
-        <f>'Cost Data'!$B94</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!F12*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="G2" s="6">
-        <f>'Cost Data'!$B94</f>
-        <v>656.31362430473212</v>
+        <f>'Pre GDP per capita adjustment'!G12*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>449.85486554705784</v>
       </c>
       <c r="H2" s="6">
-        <f>'Cost Data'!$C94</f>
-        <v>344.72326776048766</v>
+        <f>'Pre GDP per capita adjustment'!H12*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>236.28252336467378</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3370,62 +4871,64 @@
         <v>3</v>
       </c>
       <c r="B3" s="6">
-        <f>'Cost Data'!$C95</f>
-        <v>11785.714285714286</v>
+        <f>'Pre GDP per capita adjustment'!B13*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>8078.2429604331037</v>
       </c>
       <c r="C3" s="6">
-        <f>'Cost Data'!$B95</f>
-        <v>15000</v>
+        <f>'Pre GDP per capita adjustment'!C13*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>10281.400131460314</v>
       </c>
       <c r="D3" s="6">
-        <f>'Cost Data'!$B95</f>
-        <v>15000</v>
+        <f>'Pre GDP per capita adjustment'!D13*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>10281.400131460314</v>
       </c>
       <c r="E3" s="6">
-        <f>'Cost Data'!$B95</f>
-        <v>15000</v>
+        <f>'Pre GDP per capita adjustment'!E13*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>10281.400131460314</v>
       </c>
       <c r="F3" s="6">
-        <f>'Cost Data'!$B95</f>
-        <v>15000</v>
+        <f>'Pre GDP per capita adjustment'!F13*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>10281.400131460314</v>
       </c>
       <c r="G3" s="6">
-        <f>'Cost Data'!$B95</f>
-        <v>15000</v>
+        <f>'Pre GDP per capita adjustment'!G13*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>10281.400131460314</v>
       </c>
       <c r="H3" s="6">
-        <f>'Cost Data'!$C95</f>
-        <v>11785.714285714286</v>
+        <f>'Pre GDP per capita adjustment'!H13*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>8078.2429604331037</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="6">
+        <f>'Pre GDP per capita adjustment'!B14*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
       <c r="C4" s="6">
-        <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <f>'Pre GDP per capita adjustment'!C14*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
       </c>
       <c r="D4" s="6">
-        <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <f>'Pre GDP per capita adjustment'!D14*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
       </c>
       <c r="E4" s="6">
-        <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <f>'Pre GDP per capita adjustment'!E14*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
       </c>
       <c r="F4" s="6">
-        <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
+        <f>'Pre GDP per capita adjustment'!F14*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
       </c>
       <c r="G4" s="6">
-        <f>'Cost Data'!$B96</f>
-        <v>2279318.9754813975</v>
-      </c>
-      <c r="H4" s="26">
+        <f>'Pre GDP per capita adjustment'!G14*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1562306.0276102952</v>
+      </c>
+      <c r="H4" s="6">
+        <f>'Pre GDP per capita adjustment'!H14*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
     </row>
@@ -3434,62 +4937,64 @@
         <v>5</v>
       </c>
       <c r="B5" s="6">
-        <f>'Cost Data'!$C97</f>
-        <v>2434118.0622207024</v>
+        <f>'Pre GDP per capita adjustment'!B15*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1668409.4509937237</v>
       </c>
       <c r="C5" s="6">
-        <f>'Cost Data'!$B97</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!C15*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="D5" s="6">
-        <f>'Cost Data'!$B97</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!D15*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="E5" s="6">
-        <f>'Cost Data'!$B97</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!E15*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="F5" s="6">
-        <f>'Cost Data'!$B97</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!F15*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="G5" s="6">
-        <f>'Cost Data'!$B97</f>
-        <v>3332119.6733545554</v>
+        <f>'Pre GDP per capita adjustment'!G15*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>2283923.7098446013</v>
       </c>
       <c r="H5" s="6">
-        <f>'Cost Data'!$C97</f>
-        <v>2434118.0622207024</v>
+        <f>'Pre GDP per capita adjustment'!H15*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1668409.4509937237</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="6">
+        <f>'Pre GDP per capita adjustment'!B16*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
       <c r="C6" s="6">
-        <f>'Cost Data'!$B98</f>
-        <v>1695890</v>
+        <f>'Pre GDP per capita adjustment'!C16*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1162408.2445961488</v>
       </c>
       <c r="D6" s="6">
-        <f>'Cost Data'!$B98</f>
-        <v>1695890</v>
+        <f>'Pre GDP per capita adjustment'!D16*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1162408.2445961488</v>
       </c>
       <c r="E6" s="6">
-        <f>'Cost Data'!$B98</f>
-        <v>1695890</v>
+        <f>'Pre GDP per capita adjustment'!E16*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1162408.2445961488</v>
       </c>
       <c r="F6" s="6">
-        <f>'Cost Data'!$B98</f>
-        <v>1695890</v>
+        <f>'Pre GDP per capita adjustment'!F16*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1162408.2445961488</v>
       </c>
       <c r="G6" s="6">
-        <f>'Cost Data'!$B98</f>
-        <v>1695890</v>
-      </c>
-      <c r="H6" s="26">
+        <f>'Pre GDP per capita adjustment'!G16*'GDP per capita adjustmentUS Dat'!$B$15</f>
+        <v>1162408.2445961488</v>
+      </c>
+      <c r="H6" s="6">
+        <f>'Pre GDP per capita adjustment'!H16*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
     </row>
@@ -3497,25 +5002,32 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="6">
+        <f>'Pre GDP per capita adjustment'!B17*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="6">
+        <f>'Pre GDP per capita adjustment'!C17*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="6">
+        <f>'Pre GDP per capita adjustment'!D17*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="6">
+        <f>'Pre GDP per capita adjustment'!E17*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="6">
+        <f>'Pre GDP per capita adjustment'!F17*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="6">
+        <f>'Pre GDP per capita adjustment'!G17*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="6">
+        <f>'Pre GDP per capita adjustment'!H17*'GDP per capita adjustmentUS Dat'!$B$15</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes formula reference for battery electric truck maintenance cost.
</commit_message>
<xml_diff>
--- a/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
+++ b/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\AVMC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\trans\AVMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354E2386-ABE2-4A8F-9CE3-0B5B103FA882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E5E281-8241-4C04-A990-DE0FFB166F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34425" yWindow="1125" windowWidth="19185" windowHeight="14460" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1324,11 +1324,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="140"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1338,7 +1336,6 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1557,7 +1554,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Rail shipments 93-97"/>
@@ -1638,7 +1635,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="About"/>
@@ -2859,9 +2856,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2899,9 +2896,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2934,26 +2931,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2986,26 +2966,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3181,13 +3144,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="73.1796875" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3219,7 +3182,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3244,7 +3207,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3274,7 +3237,7 @@
       </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3304,7 +3267,7 @@
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3334,7 +3297,7 @@
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3364,7 +3327,7 @@
       </c>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3389,7 +3352,7 @@
       </c>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="7" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3419,7 +3382,7 @@
       </c>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3449,7 +3412,7 @@
       </c>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="7" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3479,7 +3442,7 @@
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="7" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3571,20 +3534,20 @@
       <selection activeCell="N2" sqref="N2:N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="10.81640625" customWidth="1"/>
-    <col min="13" max="13" width="10.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="11:14" s="27" customFormat="1" ht="43.5">
-      <c r="L1" s="27" t="s">
+    <row r="1" spans="11:14" s="24" customFormat="1" ht="45">
+      <c r="L1" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3646,23 +3609,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA56E7A-E0B4-48E9-AA66-C39B91D43ABA}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
@@ -3688,7 +3651,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3716,17 +3679,17 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="23" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="23" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3734,14 +3697,14 @@
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="8">
         <v>15000</v>
       </c>
       <c r="C18" t="s">
@@ -3755,7 +3718,7 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <f>6500+100*1062*3/28</f>
         <v>17878.571428571428</v>
       </c>
@@ -3770,14 +3733,14 @@
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="10">
         <v>0.28000000000000003</v>
       </c>
       <c r="C22" t="s">
@@ -3791,7 +3754,7 @@
       <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="10">
         <v>0.22</v>
       </c>
       <c r="C23" t="s">
@@ -3811,7 +3774,7 @@
       <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3819,7 +3782,7 @@
       <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="10">
         <f>$B$24*B22</f>
         <v>2595.6000000000004</v>
       </c>
@@ -3831,7 +3794,7 @@
       <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="10">
         <f>$B$24*B23</f>
         <v>2039.4</v>
       </c>
@@ -3843,7 +3806,7 @@
       <c r="A27" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="10">
         <f>B25*About!$A$77</f>
         <v>2482.986689554888</v>
       </c>
@@ -3855,7 +3818,7 @@
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <f>B26*About!$A$77</f>
         <v>1950.9181132216977</v>
       </c>
@@ -3864,20 +3827,20 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" s="12"/>
+      <c r="B29" s="10"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="11"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="14">
         <v>590</v>
       </c>
       <c r="C31" t="s">
@@ -3888,7 +3851,7 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="B32" s="16">
+      <c r="B32" s="14">
         <f>B31*About!$A$78</f>
         <v>552.6291612271541</v>
       </c>
@@ -3897,7 +3860,7 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="B33" s="18">
+      <c r="B33">
         <v>11.3</v>
       </c>
       <c r="C33" t="s">
@@ -3908,7 +3871,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="B34" s="18">
+      <c r="B34">
         <v>365</v>
       </c>
       <c r="C34" t="s">
@@ -3916,7 +3879,7 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="B35" s="16">
+      <c r="B35" s="14">
         <f>B32*B33*B34</f>
         <v>2279318.9754813975</v>
       </c>
@@ -3925,32 +3888,32 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="B36" s="16"/>
+      <c r="B36" s="14"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="11"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="16"/>
+      <c r="B38" s="14"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B39" s="16"/>
+      <c r="B39" s="14"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="10">
         <v>14.36</v>
       </c>
       <c r="C40" t="s">
@@ -3964,7 +3927,7 @@
       <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="10">
         <v>10.49</v>
       </c>
       <c r="C41" t="s">
@@ -3975,13 +3938,13 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="B42" s="16"/>
+      <c r="B42" s="14"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>102</v>
       </c>
-      <c r="B43" s="23">
+      <c r="B43" s="20">
         <f>AVERAGE(21.4,22.7,23.1,25.8,31.2)</f>
         <v>24.839999999999996</v>
       </c>
@@ -3996,7 +3959,7 @@
       <c r="A44" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="18">
+      <c r="B44">
         <f>24*365</f>
         <v>8760</v>
       </c>
@@ -4017,13 +3980,13 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="B46" s="16"/>
+      <c r="B46" s="14"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="16">
+      <c r="B47" s="14">
         <f>B40*B45</f>
         <v>3124713.0239999993</v>
       </c>
@@ -4035,7 +3998,7 @@
       <c r="A48" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="16">
+      <c r="B48" s="14">
         <f>B41*B45</f>
         <v>2282607.2159999995</v>
       </c>
@@ -4047,7 +4010,7 @@
       <c r="A49" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="16">
+      <c r="B49" s="14">
         <f>B47*About!$A$79</f>
         <v>3332119.6733545554</v>
       </c>
@@ -4059,7 +4022,7 @@
       <c r="A50" t="s">
         <v>89</v>
       </c>
-      <c r="B50" s="16">
+      <c r="B50" s="14">
         <f>B48*About!$A$79</f>
         <v>2434118.0622207024</v>
       </c>
@@ -4068,23 +4031,23 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="B51" s="16"/>
+      <c r="B51" s="14"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="B52" s="12"/>
+      <c r="B52" s="10"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="11"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="9"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="16">
+      <c r="B54" s="14">
         <v>1000</v>
       </c>
       <c r="C54" t="s">
@@ -4092,7 +4055,7 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="B55" s="16">
+      <c r="B55" s="14">
         <f>B54*About!A76</f>
         <v>914.32735845675347</v>
       </c>
@@ -4104,44 +4067,44 @@
       <c r="A56" t="s">
         <v>69</v>
       </c>
-      <c r="B56" s="12"/>
+      <c r="B56" s="10"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="12"/>
+      <c r="B57" s="10"/>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="12"/>
+      <c r="B58" s="10"/>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>72</v>
       </c>
-      <c r="B59" s="12"/>
+      <c r="B59" s="10"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="12"/>
+      <c r="B60" s="10"/>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="12"/>
+      <c r="B61" s="10"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
@@ -4152,7 +4115,7 @@
       <c r="A65" t="s">
         <v>105</v>
       </c>
-      <c r="B65" s="16">
+      <c r="B65" s="14">
         <v>1695890</v>
       </c>
       <c r="C65" t="s">
@@ -4165,17 +4128,17 @@
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="11" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4183,7 +4146,7 @@
       <c r="A71" t="s">
         <v>105</v>
       </c>
-      <c r="B71" s="24">
+      <c r="B71" s="21">
         <v>0.1</v>
       </c>
       <c r="C71" t="s">
@@ -4191,16 +4154,16 @@
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B72" s="10">
+      <c r="B72" s="8">
         <v>30000</v>
       </c>
       <c r="C72" t="s">
         <v>117</v>
       </c>
-      <c r="D72" s="13" t="s">
+      <c r="D72" s="11" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4208,7 +4171,7 @@
       <c r="A73" t="s">
         <v>105</v>
       </c>
-      <c r="B73" s="10">
+      <c r="B73" s="8">
         <f>B71*B72</f>
         <v>3000</v>
       </c>
@@ -4217,11 +4180,11 @@
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="14" t="s">
+      <c r="A78" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
     </row>
     <row r="79" spans="1:4">
       <c r="B79" s="1" t="s">
@@ -4235,11 +4198,11 @@
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="19">
+      <c r="B80" s="16">
         <f>LDVs!M2</f>
         <v>1146.6070044711444</v>
       </c>
-      <c r="C80" s="19">
+      <c r="C80" s="16">
         <f>LDVs!M4</f>
         <v>692.50522052217627</v>
       </c>
@@ -4248,11 +4211,11 @@
       <c r="A81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B81" s="19">
+      <c r="B81" s="16">
         <f>B27</f>
         <v>2482.986689554888</v>
       </c>
-      <c r="C81" s="19">
+      <c r="C81" s="16">
         <f>B28</f>
         <v>1950.9181132216977</v>
       </c>
@@ -4261,7 +4224,7 @@
       <c r="A82" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="19">
+      <c r="B82" s="16">
         <f>B35</f>
         <v>2279318.9754813975</v>
       </c>
@@ -4274,11 +4237,11 @@
       <c r="A83" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="19">
+      <c r="B83" s="16">
         <f>B49</f>
         <v>3332119.6733545554</v>
       </c>
-      <c r="C83" s="19">
+      <c r="C83" s="16">
         <f>B50</f>
         <v>2434118.0622207024</v>
       </c>
@@ -4287,7 +4250,7 @@
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B84" s="19">
+      <c r="B84" s="16">
         <f>B73</f>
         <v>3000</v>
       </c>
@@ -4300,21 +4263,21 @@
       <c r="A85" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="19">
+      <c r="B85" s="16">
         <f>B55</f>
         <v>914.32735845675347</v>
       </c>
-      <c r="C85" s="20">
+      <c r="C85" s="17">
         <f>B85*(C80/B80)</f>
         <v>552.21751352338572</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="14" t="s">
+      <c r="A87" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B87" s="15"/>
-      <c r="C87" s="15"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
     </row>
     <row r="88" spans="1:3">
       <c r="B88" s="1" t="s">
@@ -4328,11 +4291,11 @@
       <c r="A89" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B89" s="19">
+      <c r="B89" s="16">
         <f>LDVs!N2</f>
         <v>1000.4265479134275</v>
       </c>
-      <c r="C89" s="19">
+      <c r="C89" s="16">
         <f>LDVs!N4</f>
         <v>604.21801408632746</v>
       </c>
@@ -4341,11 +4304,11 @@
       <c r="A90" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B90" s="19">
+      <c r="B90" s="16">
         <f>B18</f>
         <v>15000</v>
       </c>
-      <c r="C90" s="20">
+      <c r="C90" s="17">
         <f>B90*(C81/B81)</f>
         <v>11785.714285714286</v>
       </c>
@@ -4354,7 +4317,7 @@
       <c r="A91" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B91" s="19">
+      <c r="B91" s="16">
         <f>B82</f>
         <v>2279318.9754813975</v>
       </c>
@@ -4367,11 +4330,11 @@
       <c r="A92" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="19">
+      <c r="B92" s="16">
         <f>B49</f>
         <v>3332119.6733545554</v>
       </c>
-      <c r="C92" s="19">
+      <c r="C92" s="16">
         <f>B50</f>
         <v>2434118.0622207024</v>
       </c>
@@ -4380,7 +4343,7 @@
       <c r="A93" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="19">
+      <c r="B93" s="16">
         <f>B65</f>
         <v>1695890</v>
       </c>
@@ -4421,9 +4384,9 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -5167,13 +5130,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="29">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:33" ht="30">
+      <c r="A1" s="6" t="s">
         <v>134</v>
       </c>
       <c r="B1" s="1">
@@ -6086,18 +6049,18 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
-    <col min="6" max="8" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="8" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -6192,7 +6155,7 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="22">
         <v>0</v>
       </c>
       <c r="C4" s="5">
@@ -6215,7 +6178,7 @@
         <f>'Cost Data'!$B82</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="22">
         <v>0</v>
       </c>
     </row>
@@ -6256,7 +6219,7 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="22">
         <v>0</v>
       </c>
       <c r="C6" s="5">
@@ -6279,7 +6242,7 @@
         <f>'Cost Data'!$B84</f>
         <v>3000</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <v>0</v>
       </c>
     </row>
@@ -6315,10 +6278,6 @@
         <f>'Cost Data'!$C85</f>
         <v>552.21751352338572</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" s="5"/>
@@ -6339,24 +6298,24 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
-    <col min="6" max="8" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="8" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -6385,31 +6344,31 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <f>LDVs!N4</f>
         <v>604.21801408632746</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <f>LDVs!$N$2</f>
         <v>1000.4265479134275</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <f>LDVs!$N$2</f>
         <v>1000.4265479134275</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <f>LDVs!$N$2</f>
         <v>1000.4265479134275</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>LDVs!N3</f>
         <v>891.46920111097484</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <f>LDVs!$N$2</f>
         <v>1000.4265479134275</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <f>B2</f>
         <v>604.21801408632746</v>
       </c>
@@ -6418,31 +6377,31 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6">
-        <f>'Cost Data'!B19</f>
-        <v>17878.571428571428</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="5">
+        <f>'Cost Data'!C90</f>
+        <v>11785.714285714286</v>
+      </c>
+      <c r="C3" s="5">
         <f>'Cost Data'!$B90</f>
         <v>15000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <f>'Cost Data'!$B90</f>
         <v>15000</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <f>'Cost Data'!$B90</f>
         <v>15000</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f>'Cost Data'!$B90</f>
         <v>15000</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <f>'Cost Data'!$B90</f>
         <v>15000</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f>'Cost Data'!$C90</f>
         <v>11785.714285714286</v>
       </c>
@@ -6451,30 +6410,30 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="22">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <f>'Cost Data'!$B91</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f>'Cost Data'!$B91</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <f>'Cost Data'!$B91</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f>'Cost Data'!$B91</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f>'Cost Data'!$B91</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="22">
         <v>0</v>
       </c>
     </row>
@@ -6482,31 +6441,31 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <f>'Cost Data'!$C92</f>
         <v>2434118.0622207024</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <f>'Cost Data'!$B92</f>
         <v>3332119.6733545554</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f>'Cost Data'!$B92</f>
         <v>3332119.6733545554</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <f>'Cost Data'!$B92</f>
         <v>3332119.6733545554</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f>'Cost Data'!$B92</f>
         <v>3332119.6733545554</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f>'Cost Data'!$B92</f>
         <v>3332119.6733545554</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f>'Cost Data'!$C92</f>
         <v>2434118.0622207024</v>
       </c>
@@ -6515,30 +6474,30 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="22">
         <v>0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f>'Cost Data'!$B93</f>
         <v>1695890</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f>'Cost Data'!$B93</f>
         <v>1695890</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <f>'Cost Data'!$B93</f>
         <v>1695890</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f>'Cost Data'!$B93</f>
         <v>1695890</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f>'Cost Data'!$B93</f>
         <v>1695890</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <v>0</v>
       </c>
     </row>
@@ -6546,36 +6505,27 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="22">
         <v>0</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="22">
         <v>0</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="22">
         <v>0</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>0</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="22">
         <v>0</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <v>0</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>